<commit_message>
Updated Code and Tracker
</commit_message>
<xml_diff>
--- a/08.Miscelleneous/AMIG Fraud Scenario tracker.xlsx
+++ b/08.Miscelleneous/AMIG Fraud Scenario tracker.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="44">
   <si>
     <t>Scenario</t>
   </si>
@@ -39,9 +39,6 @@
   </si>
   <si>
     <t>Multiple claim and payment done for same cause, same vendor, same amount</t>
-  </si>
-  <si>
-    <t>Check Report Date time difference</t>
   </si>
   <si>
     <t>Advisory Allowance Fraud</t>
@@ -153,10 +150,27 @@
 Also, need the external D&amp;B data to determine general contractor </t>
   </si>
   <si>
-    <t>We can not use Insured ID as there is no such column/feature as of now; We can do for Policy Number if that fulfils the requirement.  Is there any field on the contact details which uniquely defines it ?</t>
-  </si>
-  <si>
     <t>Done for claimant/receiver; We can not use Insured ID as there is no such column/feature as of now; We can do for Policy Number if that fulfils the requirement.  Is there any field on the contact details which uniquely defines it ?</t>
+  </si>
+  <si>
+    <t>Users(Managers/ Adjusters) changing the Authority Limits Frequently</t>
+  </si>
+  <si>
+    <t>a)Finding users with role as Manager
+b)Keeping Track on the change in Authority limits of the Adjusters
+c)Find users who has access to Change the Authority Limits i.e., Who has role 'User Admin' Assigned to them.</t>
+  </si>
+  <si>
+    <t>For every claim who claimed ?</t>
+  </si>
+  <si>
+    <t>Created mean and sd for the cause and decided a thresold over which there will be possibility of fraud. Then using frequency graph identify the adjustor doing it more often.</t>
+  </si>
+  <si>
+    <t>No such case in Pekin Data</t>
+  </si>
+  <si>
+    <t>Indu is working on data collection</t>
   </si>
 </sst>
 </file>
@@ -276,7 +290,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -303,6 +317,16 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -313,16 +337,13 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -656,10 +677,10 @@
   <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>
-  <dimension ref="A1:M15"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -679,7 +700,7 @@
   <sheetData>
     <row r="1" spans="1:13" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -698,26 +719,26 @@
         <v>1</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="25.2" x14ac:dyDescent="0.2">
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="18" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="9" t="s">
@@ -731,130 +752,130 @@
         <v>26</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="H5" s="17" t="s">
-        <v>5</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="H5" s="21"/>
       <c r="M5" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="25.2" x14ac:dyDescent="0.2">
-      <c r="B6" s="14"/>
+      <c r="B6" s="18"/>
       <c r="C6" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D6" s="13"/>
       <c r="E6" s="13" t="s">
         <v>3</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="H6" s="18"/>
+        <v>31</v>
+      </c>
+      <c r="H6" s="22" t="s">
+        <v>42</v>
+      </c>
       <c r="M6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="88.2" x14ac:dyDescent="0.2">
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>22</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>23</v>
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="8" t="s">
         <v>3</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="H7" s="19" t="s">
-        <v>39</v>
+        <v>31</v>
+      </c>
+      <c r="H7" s="14" t="s">
+        <v>37</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="75.599999999999994" x14ac:dyDescent="0.2">
-      <c r="B8" s="16"/>
-      <c r="C8" s="20" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="25.2" x14ac:dyDescent="0.2">
+      <c r="B8" s="20"/>
+      <c r="C8" s="15" t="s">
+        <v>23</v>
       </c>
       <c r="D8" s="8"/>
       <c r="E8" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>38</v>
+        <v>31</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>40</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="75.599999999999994" x14ac:dyDescent="0.2">
       <c r="B9" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>6</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>7</v>
       </c>
       <c r="D9" s="8"/>
       <c r="E9" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="37.799999999999997" x14ac:dyDescent="0.2">
       <c r="B10" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="8"/>
       <c r="E10" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B11" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="8"/>
@@ -862,112 +883,134 @@
         <v>3</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="H11" s="7"/>
+        <v>31</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="12" spans="1:13" ht="63" x14ac:dyDescent="0.2">
       <c r="B12" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="8"/>
       <c r="E12" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="37.799999999999997" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="63" x14ac:dyDescent="0.2">
       <c r="B13" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="8"/>
       <c r="E13" s="8" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="H13" s="7">
-        <v>4</v>
+        <v>31</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>41</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="25.2" x14ac:dyDescent="0.2">
       <c r="B14" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C14" s="7"/>
       <c r="D14" s="8"/>
       <c r="E14" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G14" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H14" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="H14" s="9" t="s">
-        <v>33</v>
-      </c>
       <c r="M14" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B15" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="8"/>
       <c r="E15" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="75.599999999999994" x14ac:dyDescent="0.2">
+      <c r="B16" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="17"/>
+      <c r="E16" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H16" s="23" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="2">
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="B7:B8"/>
-    <mergeCell ref="H5:H6"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:E15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:E16">
       <formula1>$M$4:$M$6</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F15">
       <formula1>$M$7:$M$10</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G5:G15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G5:G16">
       <formula1>$M$12:$M$14</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Update v3 Code with Images
</commit_message>
<xml_diff>
--- a/08.Miscelleneous/AMIG Fraud Scenario tracker.xlsx
+++ b/08.Miscelleneous/AMIG Fraud Scenario tracker.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19176" windowHeight="6276"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="19176" windowHeight="6276"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027" calcOnSave="0"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="51">
   <si>
     <t>Scenario</t>
   </si>
@@ -173,13 +174,25 @@
     <t>Indu is working on data collection</t>
   </si>
   <si>
-    <t>Adjustor- Receiver fraud pair</t>
-  </si>
-  <si>
     <t>Assumption</t>
   </si>
   <si>
     <t>First reserve as proxy to claimed amount</t>
+  </si>
+  <si>
+    <t>Adjustor- Receiver fraud Pair</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Insured</t>
+  </si>
+  <si>
+    <t>Claimant</t>
+  </si>
+  <si>
+    <t>Payto/Receiver</t>
   </si>
 </sst>
 </file>
@@ -350,22 +363,22 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -702,7 +715,7 @@
   <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -753,7 +766,7 @@
         <v>29</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I4" s="10" t="s">
         <v>13</v>
@@ -763,7 +776,7 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="25.2" x14ac:dyDescent="0.2">
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="20" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="7" t="s">
@@ -780,13 +793,15 @@
         <v>31</v>
       </c>
       <c r="H5" s="8"/>
-      <c r="I5" s="22"/>
+      <c r="I5" s="18" t="s">
+        <v>47</v>
+      </c>
       <c r="N5" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="25.2" x14ac:dyDescent="0.2">
-      <c r="B6" s="21"/>
+      <c r="B6" s="20"/>
       <c r="C6" s="7" t="s">
         <v>18</v>
       </c>
@@ -801,15 +816,15 @@
         <v>31</v>
       </c>
       <c r="H6" s="8"/>
-      <c r="I6" s="23" t="s">
-        <v>42</v>
+      <c r="I6" s="19" t="s">
+        <v>47</v>
       </c>
       <c r="N6" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="88.2" x14ac:dyDescent="0.2">
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="21" t="s">
         <v>21</v>
       </c>
       <c r="C7" s="7" t="s">
@@ -834,9 +849,9 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B8" s="20"/>
+      <c r="B8" s="22"/>
       <c r="C8" s="7" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D8" s="8"/>
       <c r="E8" s="8" t="s">
@@ -852,13 +867,13 @@
       <c r="I8" s="13"/>
     </row>
     <row r="9" spans="1:14" ht="25.2" x14ac:dyDescent="0.2">
-      <c r="B9" s="19"/>
+      <c r="B9" s="23"/>
       <c r="C9" s="14" t="s">
         <v>23</v>
       </c>
       <c r="D9" s="8"/>
       <c r="E9" s="8" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="F9" s="8" t="s">
         <v>28</v>
@@ -958,7 +973,7 @@
         <v>31</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I13" s="9" t="s">
         <v>35</v>
@@ -1075,4 +1090,34 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>